<commit_message>
Added RT-90 and HD1
</commit_message>
<xml_diff>
--- a/Current/Frequency_Table.xlsx
+++ b/Current/Frequency_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\Git\TURO\Current\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\johannes\src\TURO\Current\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9B0E9-AE40-4BD6-A823-E1C31CFED66B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7EDAB7-FEC8-4DD9-A5AD-EE74E760DFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -806,6 +806,9 @@
   </si>
   <si>
     <t>LPD 62</t>
+  </si>
+  <si>
+    <t>LPD 3</t>
   </si>
   <si>
     <r>
@@ -826,12 +829,9 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-https://github.com/MasterPuffin/TURO
+https://github.com/Trueforce-Defense-Inc/TURO
 Licensed under GNU General Public License v3.0</t>
     </r>
-  </si>
-  <si>
-    <t>LPD 3</t>
   </si>
 </sst>
 </file>
@@ -999,30 +999,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1044,24 +1042,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1407,7 +1402,7 @@
       <selection activeCell="C94" sqref="A1:C94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -2435,380 +2430,380 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>184</v>
       </c>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="31" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="33"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="31"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>91</v>
       </c>
       <c r="D3" s="4">
         <v>21</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>107</v>
       </c>
       <c r="G3" s="4">
         <v>52</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <v>83</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>124</v>
       </c>
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>22</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>53</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <v>84</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>123</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D5" s="4">
         <v>23</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>109</v>
       </c>
       <c r="G5" s="4">
         <v>54</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>85</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>122</v>
       </c>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>24</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>55</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <v>86</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>121</v>
       </c>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D7" s="4">
         <v>25</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>110</v>
       </c>
       <c r="G7" s="4">
         <v>56</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>87</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>120</v>
       </c>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>26</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>57</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <v>88</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>119</v>
       </c>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>97</v>
       </c>
       <c r="D9" s="4">
         <v>27</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>135</v>
       </c>
       <c r="G9" s="4">
         <v>58</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>89</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="5" t="s">
         <v>118</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>28</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>59</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>167</v>
       </c>
       <c r="J10" s="2"/>
@@ -2817,31 +2812,31 @@
       <c r="M10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D11" s="4">
         <v>29</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>137</v>
       </c>
       <c r="G11" s="4">
         <v>60</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>168</v>
       </c>
       <c r="J11" s="2"/>
@@ -2850,31 +2845,31 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>30</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>61</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>169</v>
       </c>
       <c r="J12" s="2"/>
@@ -2883,31 +2878,31 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>101</v>
       </c>
       <c r="D13" s="4">
         <v>31</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G13" s="4">
         <v>62</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>170</v>
       </c>
       <c r="J13" s="2"/>
@@ -2916,31 +2911,31 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>32</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>63</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>171</v>
       </c>
       <c r="J14" s="2"/>
@@ -2949,31 +2944,31 @@
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>103</v>
       </c>
       <c r="D15" s="4">
         <v>33</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>141</v>
       </c>
       <c r="G15" s="4">
         <v>64</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>172</v>
       </c>
       <c r="J15" s="2"/>
@@ -2982,114 +2977,114 @@
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>34</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>65</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>105</v>
       </c>
       <c r="D17" s="4">
         <v>35</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>143</v>
       </c>
       <c r="G17" s="4">
         <v>66</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <v>91</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="5" t="s">
         <v>117</v>
       </c>
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>36</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>67</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="10">
         <v>92</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="K18" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="9" t="s">
         <v>116</v>
       </c>
       <c r="M18" s="2"/>
@@ -3098,31 +3093,31 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>37</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>145</v>
       </c>
       <c r="G19" s="4">
         <v>68</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="6">
         <v>93</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="5" t="s">
         <v>115</v>
       </c>
       <c r="M19" s="2"/>
@@ -3131,31 +3126,31 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="11">
+      <c r="D20" s="10">
         <v>38</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>69</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="10">
         <v>94</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="9" t="s">
         <v>114</v>
       </c>
       <c r="M20" s="2"/>
@@ -3164,31 +3159,31 @@
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>39</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>147</v>
       </c>
       <c r="G21" s="4">
         <v>70</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>95</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="5" t="s">
         <v>113</v>
       </c>
       <c r="M21" s="2"/>
@@ -3197,52 +3192,52 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="11">
+      <c r="D22" s="10">
         <v>40</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>71</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="10">
         <v>96</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="L22" s="9" t="s">
         <v>112</v>
       </c>
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>41</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>149</v>
       </c>
       <c r="G23" s="4">
         <v>72</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>180</v>
       </c>
       <c r="J23" s="2"/>
@@ -3251,109 +3246,109 @@
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="D24" s="11">
+      <c r="B24" s="26"/>
+      <c r="D24" s="10">
         <v>42</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <v>73</v>
       </c>
-      <c r="H24" s="9" t="s">
+      <c r="H24" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="9" t="s">
         <v>181</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="7">
+      <c r="C25" s="14"/>
+      <c r="D25" s="6">
         <v>43</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>151</v>
       </c>
       <c r="G25" s="4">
         <v>74</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="5" t="s">
         <v>133</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="11">
+      <c r="C26" s="14"/>
+      <c r="D26" s="10">
         <v>44</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="7">
         <v>75</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="9" t="s">
         <v>132</v>
       </c>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>45</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>153</v>
       </c>
       <c r="G27" s="4">
         <v>76</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="5" t="s">
         <v>131</v>
       </c>
       <c r="J27" s="2"/>
@@ -3362,159 +3357,159 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="11">
+      <c r="D28" s="10">
         <v>46</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <v>77</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="9" t="s">
         <v>130</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="20"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="19"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>47</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>155</v>
       </c>
       <c r="G29" s="4">
         <v>78</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="5" t="s">
         <v>129</v>
       </c>
       <c r="J29" s="2"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="22"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="11">
+      <c r="D30" s="10">
         <v>48</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="7">
         <v>79</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="I30" s="9" t="s">
         <v>128</v>
       </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="L30" s="24"/>
+      <c r="K30" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="L30" s="22"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>49</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>157</v>
       </c>
       <c r="G31" s="4">
         <v>80</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="5" t="s">
         <v>127</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="22"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="11">
+      <c r="D32" s="10">
         <v>50</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="G32" s="8">
+      <c r="G32" s="7">
         <v>81</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="9" t="s">
         <v>126</v>
       </c>
       <c r="J32" s="2"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="26"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="24"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>51</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>159</v>
       </c>
       <c r="G33" s="4">
         <v>82</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="5" t="s">
         <v>125</v>
       </c>
       <c r="J33" s="2"/>
-      <c r="L33" s="18"/>
+      <c r="L33" s="17"/>
       <c r="M33" s="2"/>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>